<commit_message>
thermal pva table added
</commit_message>
<xml_diff>
--- a/Backend/templates/uwa.xlsx
+++ b/Backend/templates/uwa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\react projects\nokia\Nokia-DWS-main\Backend\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\react projects\nokia\new-nokia\Backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB7BCE3-B78D-4DD9-8063-D488C19BD3FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3735D1DF-1B58-49AC-8580-7DA5738F2694}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Approver</t>
+  </si>
+  <si>
+    <t>Document ID</t>
+  </si>
+  <si>
+    <t>Document location</t>
+  </si>
+  <si>
+    <t>P.Nithiyakalyanam</t>
+  </si>
+  <si>
+    <t>MO Chennai Factory</t>
+  </si>
+  <si>
+    <t>Ramakrishna Patra</t>
+  </si>
+  <si>
+    <t>D524865660</t>
+  </si>
+  <si>
+    <t>https://sharenet-ims.inside.nokiasiemensnetworks.com/Guest/Overview/D524865660</t>
+  </si>
   <si>
     <t>Change History</t>
   </si>
@@ -33,62 +66,77 @@
     <t>For Internal Use</t>
   </si>
   <si>
-    <t>14-03-2018 - MMILPTPIT232-895545559-126 - 1.0</t>
-  </si>
-  <si>
-    <t>Testers Checklist UWA</t>
-  </si>
-  <si>
-    <t>Checked By</t>
+    <t>06-04-2016 - D524865660 - 4.0</t>
+  </si>
+  <si>
+    <t>This material, including documentation and any related computer programs, is protected by copyright controlled by Nokia Solutions and Networks. All rights are reserved. Copying, including reproducing, storing, adapting or translating, any or all of this material requires the prior written consent of  Nokia Solutions and Networks. This material also contains confidential information, which may not  be disclosed to others without the prior written consent of Nokia Solutions and Networks.</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
   <si>
     <t>Shift</t>
   </si>
   <si>
-    <t>Date</t>
+    <t>Machine Sl No</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>UWA1</t>
-  </si>
-  <si>
-    <t>UWA2</t>
-  </si>
-  <si>
-    <t>UWA3</t>
-  </si>
-  <si>
-    <t>UWA4</t>
-  </si>
-  <si>
-    <t>UWA5</t>
-  </si>
-  <si>
-    <t>UWA6</t>
-  </si>
-  <si>
-    <t>UWA7</t>
-  </si>
-  <si>
-    <t>UWA8</t>
-  </si>
-  <si>
-    <t>UWA9</t>
-  </si>
-  <si>
-    <t>UWA10</t>
-  </si>
-  <si>
-    <t>Status</t>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>UWA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uwa1 </t>
+  </si>
+  <si>
+    <t>Uwa2</t>
+  </si>
+  <si>
+    <t>Uwa3</t>
+  </si>
+  <si>
+    <t>Uwa4</t>
+  </si>
+  <si>
+    <t>Uwa5</t>
+  </si>
+  <si>
+    <t>Uwa6</t>
+  </si>
+  <si>
+    <t>Uwa7</t>
+  </si>
+  <si>
+    <t>Uwa8</t>
+  </si>
+  <si>
+    <t>Uwa9</t>
+  </si>
+  <si>
+    <t>Uwa10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +169,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -145,16 +208,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -163,15 +226,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -189,7 +258,26 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -513,155 +601,372 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="C9" s="1"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="4" t="s">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="2"/>
+    </row>
+    <row r="20" spans="1:27" ht="15" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="O14" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="D20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="W20" s="6"/>
+      <c r="X20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA20" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="W21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="15">
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:Q20"/>
     <mergeCell ref="A1:D4"/>
     <mergeCell ref="A7:E8"/>
-    <mergeCell ref="A11:D12"/>
+    <mergeCell ref="A17:D18"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D19:U19"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="L10:T15"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="T20:U20"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <conditionalFormatting sqref="A22:N1048576 A21:W21">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A21&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C15" r:id="rId1" xr:uid="{37FAF1AC-5547-4C8B-B53B-377EACF0DB70}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>